<commit_message>
Sorted some things out
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BenDa\Desktop\Code\schedule_helper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\Code\schedule_helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8ED628-934E-4BF0-AA88-A7A2CA658080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B23223-99B3-4E38-B4D2-BA1B0C989373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -171,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -197,6 +197,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -505,7 +508,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -515,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,6 +560,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="11">
+        <v>0.29583333333333334</v>
+      </c>
+    </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
         <v>6</v>
@@ -626,6 +634,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="11">
+        <v>0.29583333333333334</v>
+      </c>
+    </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" s="6" t="s">
         <v>6</v>
@@ -695,6 +708,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="11">
+        <v>0.29583333333333334</v>
+      </c>
+    </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27" s="6" t="s">
         <v>6</v>
@@ -764,6 +782,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="11">
+        <v>0.29583333333333334</v>
+      </c>
+    </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C38" s="6" t="s">
         <v>6</v>
@@ -833,6 +856,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="11">
+        <v>0.29583333333333334</v>
+      </c>
+    </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C49" s="6" t="s">
         <v>6</v>
@@ -902,6 +930,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="11">
+        <v>0.29583333333333334</v>
+      </c>
+    </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C60" s="6" t="s">
         <v>6</v>
@@ -969,6 +1002,11 @@
       </c>
       <c r="D69" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="11">
+        <v>0.29583333333333334</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Development complete ahead of refactoring
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\Code\schedule_helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883E15DF-1A45-4E73-A8DC-632E92029AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955DF9DD-3731-4836-A6C4-0EEE158F2210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="4170" windowWidth="13500" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-5595" windowWidth="18240" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -198,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -238,6 +238,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,8 +644,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="C12" s="1"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -717,8 +719,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="C23" s="1"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -791,8 +794,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="C34" s="1"/>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -872,232 +876,235 @@
       <c r="C46" s="1"/>
     </row>
     <row r="47" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="B48" s="14" t="s">
+      <c r="B47" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="14"/>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="C47" s="15"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B48" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D48" s="12" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" s="3" t="s">
+      <c r="D50" s="11">
+        <v>0.29583333333333334</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="9"/>
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="D60" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D51" s="11">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="11">
         <v>0.29583333333333334</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="6" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="7" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C64" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="8" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" s="3" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B60" s="10" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="9"/>
+      <c r="C69" s="3"/>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D60" s="12" t="s">
+      <c r="D70" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" s="3" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="D71" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D62" s="11">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="11">
         <v>0.29583333333333334</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C63" s="6" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C73" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C64" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="7" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C75" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C67" s="8" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C69" s="3" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="C70" s="1"/>
-    </row>
-    <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D73" s="11">
-        <v>0.29583333333333334</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A80" s="9"/>
+      <c r="C80" s="3"/>
     </row>
     <row r="81" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
@@ -1171,9 +1178,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B48:C48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>